<commit_message>
add img for testing
</commit_message>
<xml_diff>
--- a/sheet/CONTROLE_DE_TERRITORIO_2022.xlsx
+++ b/sheet/CONTROLE_DE_TERRITORIO_2022.xlsx
@@ -15,7 +15,7 @@
     <sheet name="NOVA" sheetId="3" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">NOVA!$A$1:$K$64</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">NOVA!$A$1:$K$66</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="40">
   <si>
     <t>OK</t>
   </si>
@@ -1299,10 +1299,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:L64"/>
+  <dimension ref="A1:L66"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="99" zoomScaleNormal="100" zoomScalePageLayoutView="45" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="99" zoomScaleNormal="100" zoomScalePageLayoutView="45" workbookViewId="0">
+      <selection activeCell="I65" sqref="I65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3169,10 +3169,12 @@
       <c r="L60" s="36"/>
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A61" s="33">
+      <c r="A61" s="80">
         <v>42</v>
       </c>
-      <c r="B61" s="10"/>
+      <c r="B61" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="C61" s="19">
         <v>44822</v>
       </c>
@@ -3189,108 +3191,182 @@
       <c r="H61" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="I61" s="27" t="s">
+      <c r="I61" s="76" t="s">
+        <v>4</v>
+      </c>
+      <c r="J61" s="78">
+        <v>41</v>
+      </c>
+      <c r="K61" s="78">
+        <v>3</v>
+      </c>
+      <c r="L61" s="74"/>
+    </row>
+    <row r="62" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="81"/>
+      <c r="B62" s="58" t="s">
+        <v>26</v>
+      </c>
+      <c r="C62" s="19">
+        <v>44839</v>
+      </c>
+      <c r="D62" s="19"/>
+      <c r="E62" s="20">
+        <v>44839</v>
+      </c>
+      <c r="F62" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="G62" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="H62" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="I62" s="77"/>
+      <c r="J62" s="79"/>
+      <c r="K62" s="79"/>
+      <c r="L62" s="75"/>
+    </row>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A63" s="85">
+        <v>43</v>
+      </c>
+      <c r="B63" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C63" s="22">
+        <v>44815</v>
+      </c>
+      <c r="D63" s="22">
+        <f t="shared" ref="D63" si="1">C63+7</f>
+        <v>44822</v>
+      </c>
+      <c r="E63" s="23">
+        <v>44822</v>
+      </c>
+      <c r="F63" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="G63" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="H63" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="I63" s="76" t="s">
+        <v>4</v>
+      </c>
+      <c r="J63" s="87">
+        <v>57</v>
+      </c>
+      <c r="K63" s="87">
+        <v>4</v>
+      </c>
+      <c r="L63" s="89"/>
+    </row>
+    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A64" s="86"/>
+      <c r="B64" s="57" t="s">
+        <v>26</v>
+      </c>
+      <c r="C64" s="22">
+        <v>44839</v>
+      </c>
+      <c r="D64" s="22"/>
+      <c r="E64" s="23">
+        <v>44839</v>
+      </c>
+      <c r="F64" s="24" t="s">
+        <v>24</v>
+      </c>
+      <c r="G64" s="25" t="s">
+        <v>2</v>
+      </c>
+      <c r="H64" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="I64" s="77"/>
+      <c r="J64" s="88"/>
+      <c r="K64" s="88"/>
+      <c r="L64" s="90"/>
+    </row>
+    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A65" s="33">
+        <v>44</v>
+      </c>
+      <c r="B65" s="10"/>
+      <c r="C65" s="19">
+        <v>44839</v>
+      </c>
+      <c r="D65" s="19"/>
+      <c r="E65" s="20">
+        <v>44839</v>
+      </c>
+      <c r="F65" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="G65" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="H65" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="I65" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="J65" s="10">
+        <v>38</v>
+      </c>
+      <c r="K65" s="10">
+        <v>3</v>
+      </c>
+      <c r="L65" s="34"/>
+    </row>
+    <row r="66" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A66" s="37">
+        <v>45</v>
+      </c>
+      <c r="B66" s="38"/>
+      <c r="C66" s="39">
+        <v>44829</v>
+      </c>
+      <c r="D66" s="39"/>
+      <c r="E66" s="40">
+        <v>44829</v>
+      </c>
+      <c r="F66" s="41" t="s">
+        <v>10</v>
+      </c>
+      <c r="G66" s="42" t="s">
+        <v>9</v>
+      </c>
+      <c r="H66" s="42" t="s">
+        <v>11</v>
+      </c>
+      <c r="I66" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="J61" s="10">
-        <v>41</v>
-      </c>
-      <c r="K61" s="10">
+      <c r="J66" s="44">
+        <v>53</v>
+      </c>
+      <c r="K66" s="44">
         <v>3</v>
       </c>
-      <c r="L61" s="34"/>
-    </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A62" s="30">
-        <v>43</v>
-      </c>
-      <c r="B62" s="9"/>
-      <c r="C62" s="22">
-        <v>44815</v>
-      </c>
-      <c r="D62" s="22">
-        <f t="shared" ref="D62" si="1">C62+7</f>
-        <v>44822</v>
-      </c>
-      <c r="E62" s="23">
-        <v>44822</v>
-      </c>
-      <c r="F62" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="G62" s="25" t="s">
-        <v>9</v>
-      </c>
-      <c r="H62" s="25" t="s">
-        <v>11</v>
-      </c>
-      <c r="I62" s="27" t="s">
-        <v>0</v>
-      </c>
-      <c r="J62" s="8">
-        <v>57</v>
-      </c>
-      <c r="K62" s="8">
-        <v>4</v>
-      </c>
-      <c r="L62" s="29"/>
-    </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A63" s="33">
-        <v>44</v>
-      </c>
-      <c r="B63" s="10"/>
-      <c r="C63" s="19"/>
-      <c r="D63" s="19"/>
-      <c r="E63" s="20"/>
-      <c r="F63" s="21"/>
-      <c r="G63" s="10"/>
-      <c r="H63" s="10"/>
-      <c r="I63" s="27" t="s">
-        <v>0</v>
-      </c>
-      <c r="J63" s="10">
-        <v>38</v>
-      </c>
-      <c r="K63" s="10">
-        <v>3</v>
-      </c>
-      <c r="L63" s="34"/>
-    </row>
-    <row r="64" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="37">
-        <v>45</v>
-      </c>
-      <c r="B64" s="38"/>
-      <c r="C64" s="39">
-        <v>44829</v>
-      </c>
-      <c r="D64" s="39"/>
-      <c r="E64" s="40">
-        <v>44829</v>
-      </c>
-      <c r="F64" s="41" t="s">
-        <v>10</v>
-      </c>
-      <c r="G64" s="42" t="s">
-        <v>9</v>
-      </c>
-      <c r="H64" s="42" t="s">
-        <v>11</v>
-      </c>
-      <c r="I64" s="43" t="s">
-        <v>0</v>
-      </c>
-      <c r="J64" s="44">
-        <v>53</v>
-      </c>
-      <c r="K64" s="44">
-        <v>3</v>
-      </c>
-      <c r="L64" s="45"/>
+      <c r="L66" s="45"/>
     </row>
   </sheetData>
-  <mergeCells count="80">
+  <mergeCells count="90">
+    <mergeCell ref="L61:L62"/>
+    <mergeCell ref="A63:A64"/>
+    <mergeCell ref="I63:I64"/>
+    <mergeCell ref="J63:J64"/>
+    <mergeCell ref="K63:K64"/>
+    <mergeCell ref="L63:L64"/>
+    <mergeCell ref="A61:A62"/>
+    <mergeCell ref="I61:I62"/>
+    <mergeCell ref="J61:J62"/>
+    <mergeCell ref="K61:K62"/>
     <mergeCell ref="J52:J53"/>
     <mergeCell ref="K52:K53"/>
     <mergeCell ref="L52:L53"/>

</xml_diff>